<commit_message>
Show number of people in studies
LF-2820
</commit_message>
<xml_diff>
--- a/src/conf/xlsx/column-and-parameter-descriptions-R5.xlsx
+++ b/src/conf/xlsx/column-and-parameter-descriptions-R5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\lhc-lx-sedinkinya\sedinkinya\Projects\fhir-obs-viewer\src\conf\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200BF475-A203-4E9B-B8EE-3F1D35479467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9B4076-969B-4FF1-B5B5-3EDE1588AC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2490" yWindow="2190" windowWidth="38700" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6570" yWindow="2865" windowWidth="38700" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources on LForms R5 server" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8708" uniqueCount="1615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8722" uniqueCount="1619">
   <si>
     <t>Legend</t>
   </si>
@@ -4866,6 +4866,18 @@
   </si>
   <si>
     <t>disable</t>
+  </si>
+  <si>
+    <t>Actual total number of participants enrolled in study</t>
+  </si>
+  <si>
+    <t>unsignedInt</t>
+  </si>
+  <si>
+    <t># of participants</t>
+  </si>
+  <si>
+    <t>recruitment.actualNumber</t>
   </si>
 </sst>
 </file>
@@ -5280,10 +5292,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H328"/>
+  <dimension ref="A1:H329"/>
   <sheetViews>
-    <sheetView topLeftCell="A170" workbookViewId="0">
-      <selection activeCell="E203" sqref="E203"/>
+    <sheetView topLeftCell="A294" workbookViewId="0">
+      <selection activeCell="A312" sqref="A312:XFD312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -11850,37 +11862,39 @@
       </c>
     </row>
     <row r="312" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A312" s="6"/>
-      <c r="B312" s="6" t="s">
+      <c r="A312" s="2"/>
+      <c r="B312" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="C312" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D312" s="6" t="s">
-        <v>613</v>
-      </c>
-      <c r="E312" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F312" s="7" t="s">
-        <v>614</v>
-      </c>
-      <c r="G312" s="6"/>
-      <c r="H312" s="6" t="s">
-        <v>615</v>
+      <c r="C312" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D312" s="2" t="s">
+        <v>1617</v>
+      </c>
+      <c r="E312" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F312" s="2" t="s">
+        <v>1616</v>
+      </c>
+      <c r="G312" s="2" t="s">
+        <v>1618</v>
+      </c>
+      <c r="H312" s="2" t="s">
+        <v>1615</v>
       </c>
     </row>
     <row r="313" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A313" s="6"/>
       <c r="B313" s="6" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="C313" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D313" s="6" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="E313" s="6" t="s">
         <v>19</v>
@@ -11890,336 +11904,358 @@
       </c>
       <c r="G313" s="6"/>
       <c r="H313" s="6" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="314" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A314" s="6"/>
       <c r="B314" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C314" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D314" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E314" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F314" s="7" t="s">
-        <v>35</v>
+        <v>614</v>
       </c>
       <c r="G314" s="6"/>
       <c r="H314" s="6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="315" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A315" s="8"/>
-      <c r="B315" s="8" t="s">
+      <c r="A315" s="6"/>
+      <c r="B315" s="6" t="s">
         <v>618</v>
       </c>
-      <c r="C315" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D315" s="8" t="s">
-        <v>620</v>
-      </c>
-      <c r="E315" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F315" s="9" t="s">
+      <c r="C315" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D315" s="6" t="s">
+        <v>618</v>
+      </c>
+      <c r="E315" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F315" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G315" s="8"/>
-      <c r="H315" s="8" t="s">
+      <c r="G315" s="6"/>
+      <c r="H315" s="6" t="s">
         <v>619</v>
       </c>
     </row>
     <row r="316" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A316" s="8"/>
       <c r="B316" s="8" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="C316" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D316" s="8" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E316" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F316" s="12" t="s">
-        <v>623</v>
+      <c r="F316" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="G316" s="8"/>
       <c r="H316" s="8" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
     </row>
     <row r="317" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A317" s="8"/>
       <c r="B317" s="8" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="C317" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D317" s="8" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="E317" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F317" s="9" t="s">
-        <v>56</v>
+      <c r="F317" s="12" t="s">
+        <v>623</v>
       </c>
       <c r="G317" s="8"/>
       <c r="H317" s="8" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A318" s="8"/>
+      <c r="B318" s="8" t="s">
+        <v>625</v>
+      </c>
+      <c r="C318" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D318" s="8" t="s">
+        <v>626</v>
+      </c>
+      <c r="E318" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F318" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G318" s="8"/>
+      <c r="H318" s="8" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A318" s="6"/>
-      <c r="B318" s="6" t="s">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A319" s="6"/>
+      <c r="B319" s="6" t="s">
         <v>628</v>
       </c>
-      <c r="C318" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D318" s="6" t="s">
+      <c r="C319" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D319" s="6" t="s">
         <v>628</v>
       </c>
-      <c r="E318" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F318" s="7" t="s">
+      <c r="E319" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F319" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="G318" s="6"/>
-      <c r="H318" s="6" t="s">
+      <c r="G319" s="6"/>
+      <c r="H319" s="6" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A319" s="8"/>
-      <c r="B319" s="8" t="s">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A320" s="8"/>
+      <c r="B320" s="8" t="s">
         <v>628</v>
       </c>
-      <c r="C319" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D319" s="8" t="s">
+      <c r="C320" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D320" s="8" t="s">
         <v>630</v>
       </c>
-      <c r="E319" s="8" t="s">
+      <c r="E320" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F319" s="9" t="s">
+      <c r="F320" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="G319" s="8"/>
-      <c r="H319" s="8" t="s">
+      <c r="G320" s="8"/>
+      <c r="H320" s="8" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A320" s="6"/>
-      <c r="B320" s="6" t="s">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A321" s="6"/>
+      <c r="B321" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="C320" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D320" s="6" t="s">
+      <c r="C321" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D321" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E320" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F320" s="7" t="s">
+      <c r="E321" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F321" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G320" s="6"/>
-      <c r="H320" s="6" t="s">
+      <c r="G321" s="6"/>
+      <c r="H321" s="6" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A321" s="10"/>
-      <c r="B321" s="10" t="s">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A322" s="10"/>
+      <c r="B322" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="C321" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D321" s="10" t="s">
+      <c r="C322" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D322" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="E321" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F321" s="11" t="s">
+      <c r="E322" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F322" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="G321" s="10"/>
-      <c r="H321" s="10" t="s">
+      <c r="G322" s="10"/>
+      <c r="H322" s="10" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A322" s="6"/>
-      <c r="B322" s="6" t="s">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A323" s="6"/>
+      <c r="B323" s="6" t="s">
         <v>633</v>
       </c>
-      <c r="C322" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D322" s="6" t="s">
+      <c r="C323" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D323" s="6" t="s">
         <v>633</v>
       </c>
-      <c r="E322" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F322" s="7" t="s">
+      <c r="E323" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F323" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G322" s="6"/>
-      <c r="H322" s="6" t="s">
+      <c r="G323" s="6"/>
+      <c r="H323" s="6" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A323" s="8"/>
-      <c r="B323" s="8" t="s">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A324" s="8"/>
+      <c r="B324" s="8" t="s">
         <v>635</v>
       </c>
-      <c r="C323" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D323" s="8" t="s">
+      <c r="C324" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D324" s="8" t="s">
         <v>636</v>
       </c>
-      <c r="E323" s="8" t="s">
+      <c r="E324" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F323" s="9" t="s">
+      <c r="F324" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G323" s="8"/>
-      <c r="H323" s="8" t="s">
+      <c r="G324" s="8"/>
+      <c r="H324" s="8" t="s">
         <v>634</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A324" s="6"/>
-      <c r="B324" s="6" t="s">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A325" s="6"/>
+      <c r="B325" s="6" t="s">
         <v>637</v>
       </c>
-      <c r="C324" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D324" s="6" t="s">
+      <c r="C325" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D325" s="6" t="s">
         <v>637</v>
       </c>
-      <c r="E324" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F324" s="7" t="s">
+      <c r="E325" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F325" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G324" s="6"/>
-      <c r="H324" s="6" t="s">
+      <c r="G325" s="6"/>
+      <c r="H325" s="6" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A325" s="10"/>
-      <c r="B325" s="10" t="s">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A326" s="10"/>
+      <c r="B326" s="10" t="s">
         <v>637</v>
       </c>
-      <c r="C325" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D325" s="10" t="s">
+      <c r="C326" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D326" s="10" t="s">
         <v>639</v>
       </c>
-      <c r="E325" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F325" s="11" t="s">
+      <c r="E326" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F326" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G325" s="10"/>
-      <c r="H325" s="10" t="s">
+      <c r="G326" s="10"/>
+      <c r="H326" s="10" t="s">
         <v>640</v>
-      </c>
-    </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A326" s="8"/>
-      <c r="B326" s="8" t="s">
-        <v>641</v>
-      </c>
-      <c r="C326" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D326" s="8" t="s">
-        <v>642</v>
-      </c>
-      <c r="E326" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F326" s="9" t="s">
-        <v>366</v>
-      </c>
-      <c r="G326" s="8"/>
-      <c r="H326" s="8" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="327" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A327" s="8"/>
       <c r="B327" s="8" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="C327" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D327" s="8" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="E327" s="8" t="s">
         <v>31</v>
       </c>
       <c r="F327" s="9" t="s">
-        <v>26</v>
+        <v>366</v>
       </c>
       <c r="G327" s="8"/>
       <c r="H327" s="8" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="328" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A328" s="8"/>
       <c r="B328" s="8" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="C328" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D328" s="8" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="E328" s="8" t="s">
         <v>31</v>
       </c>
       <c r="F328" s="9" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="G328" s="8"/>
       <c r="H328" s="8" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A329" s="8"/>
+      <c r="B329" s="8" t="s">
+        <v>647</v>
+      </c>
+      <c r="C329" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D329" s="8" t="s">
+        <v>648</v>
+      </c>
+      <c r="E329" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F329" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G329" s="8"/>
+      <c r="H329" s="8" t="s">
         <v>649</v>
       </c>
     </row>
@@ -12230,10 +12266,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H1171"/>
+  <dimension ref="A1:H1172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A1042" workbookViewId="0">
+      <selection activeCell="G1069" sqref="G1069"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -35141,37 +35177,39 @@
       </c>
     </row>
     <row r="1069" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1069" s="6"/>
-      <c r="B1069" s="6" t="s">
+      <c r="A1069" s="2"/>
+      <c r="B1069" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="C1069" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1069" s="6" t="s">
-        <v>613</v>
-      </c>
-      <c r="E1069" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1069" s="7" t="s">
-        <v>614</v>
-      </c>
-      <c r="G1069" s="6"/>
-      <c r="H1069" s="6" t="s">
-        <v>615</v>
+      <c r="C1069" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1069" s="2" t="s">
+        <v>1617</v>
+      </c>
+      <c r="E1069" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1069" s="2" t="s">
+        <v>1616</v>
+      </c>
+      <c r="G1069" s="2" t="s">
+        <v>1618</v>
+      </c>
+      <c r="H1069" s="2" t="s">
+        <v>1615</v>
       </c>
     </row>
     <row r="1070" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1070" s="6"/>
       <c r="B1070" s="6" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="C1070" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D1070" s="6" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="E1070" s="6" t="s">
         <v>19</v>
@@ -35181,29 +35219,29 @@
       </c>
       <c r="G1070" s="6"/>
       <c r="H1070" s="6" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="1071" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1071" s="6"/>
       <c r="B1071" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C1071" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D1071" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E1071" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1071" s="7" t="s">
-        <v>35</v>
+        <v>614</v>
       </c>
       <c r="G1071" s="6"/>
       <c r="H1071" s="6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="1072" spans="1:8" x14ac:dyDescent="0.25">
@@ -35212,10 +35250,10 @@
         <v>618</v>
       </c>
       <c r="C1072" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1072" s="6" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="E1072" s="6" t="s">
         <v>19</v>
@@ -35231,67 +35269,67 @@
     <row r="1073" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1073" s="6"/>
       <c r="B1073" s="6" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="C1073" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1073" s="6" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E1073" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1073" s="12" t="s">
-        <v>623</v>
+        <v>19</v>
+      </c>
+      <c r="F1073" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="G1073" s="6"/>
       <c r="H1073" s="6" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
     </row>
     <row r="1074" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1074" s="6"/>
       <c r="B1074" s="6" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="C1074" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1074" s="6" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="E1074" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1074" s="7" t="s">
-        <v>56</v>
+        <v>31</v>
+      </c>
+      <c r="F1074" s="12" t="s">
+        <v>623</v>
       </c>
       <c r="G1074" s="6"/>
       <c r="H1074" s="6" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="1075" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1075" s="6"/>
       <c r="B1075" s="6" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="C1075" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1075" s="6" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="E1075" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1075" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G1075" s="6"/>
       <c r="H1075" s="6" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="1076" spans="1:8" x14ac:dyDescent="0.25">
@@ -35300,16 +35338,16 @@
         <v>628</v>
       </c>
       <c r="C1076" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1076" s="6" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="E1076" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1076" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G1076" s="6"/>
       <c r="H1076" s="6" t="s">
@@ -35319,23 +35357,23 @@
     <row r="1077" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1077" s="6"/>
       <c r="B1077" s="6" t="s">
-        <v>215</v>
+        <v>628</v>
       </c>
       <c r="C1077" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1077" s="6" t="s">
-        <v>215</v>
+        <v>630</v>
       </c>
       <c r="E1077" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1077" s="7" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G1077" s="6"/>
       <c r="H1077" s="6" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="1078" spans="1:8" x14ac:dyDescent="0.25">
@@ -35344,10 +35382,10 @@
         <v>215</v>
       </c>
       <c r="C1078" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1078" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E1078" s="6" t="s">
         <v>19</v>
@@ -35357,41 +35395,41 @@
       </c>
       <c r="G1078" s="6"/>
       <c r="H1078" s="6" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="1079" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1079" s="6"/>
       <c r="B1079" s="6" t="s">
-        <v>633</v>
+        <v>215</v>
       </c>
       <c r="C1079" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1079" s="6" t="s">
-        <v>633</v>
+        <v>217</v>
       </c>
       <c r="E1079" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1079" s="7" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="G1079" s="6"/>
       <c r="H1079" s="6" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="1080" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1080" s="6"/>
       <c r="B1080" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="C1080" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1080" s="6" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="E1080" s="6" t="s">
         <v>19</v>
@@ -35407,23 +35445,23 @@
     <row r="1081" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1081" s="6"/>
       <c r="B1081" s="6" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C1081" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1081" s="6" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E1081" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1081" s="7" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="G1081" s="6"/>
       <c r="H1081" s="6" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
     </row>
     <row r="1082" spans="1:8" x14ac:dyDescent="0.25">
@@ -35432,10 +35470,10 @@
         <v>637</v>
       </c>
       <c r="C1082" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1082" s="6" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="E1082" s="6" t="s">
         <v>19</v>
@@ -35445,112 +35483,112 @@
       </c>
       <c r="G1082" s="6"/>
       <c r="H1082" s="6" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="1083" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1083" s="6"/>
       <c r="B1083" s="6" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="C1083" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1083" s="6" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="E1083" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1083" s="7" t="s">
-        <v>366</v>
+        <v>26</v>
       </c>
       <c r="G1083" s="6"/>
       <c r="H1083" s="6" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="1084" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1084" s="6"/>
       <c r="B1084" s="6" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="C1084" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1084" s="6" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="E1084" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1084" s="7" t="s">
-        <v>26</v>
+        <v>366</v>
       </c>
       <c r="G1084" s="6"/>
       <c r="H1084" s="6" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="1085" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1085" s="6"/>
       <c r="B1085" s="6" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="C1085" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1085" s="6" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
       <c r="E1085" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1085" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="G1085" s="6"/>
       <c r="H1085" s="6" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1086" s="6"/>
+      <c r="B1086" s="6" t="s">
+        <v>647</v>
+      </c>
+      <c r="C1086" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1086" s="6" t="s">
+        <v>648</v>
+      </c>
+      <c r="E1086" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1086" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1086" s="6"/>
+      <c r="H1086" s="6" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="1086" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1086" t="s">
+    <row r="1087" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1087" t="s">
         <v>1543</v>
-      </c>
-    </row>
-    <row r="1087" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1087" s="6"/>
-      <c r="B1087" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C1087" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1087" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="E1087" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1087" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1087" s="6"/>
-      <c r="H1087" s="6" t="s">
-        <v>1544</v>
       </c>
     </row>
     <row r="1088" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1088" s="6"/>
       <c r="B1088" s="6" t="s">
-        <v>1545</v>
+        <v>129</v>
       </c>
       <c r="C1088" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1088" s="6" t="s">
-        <v>1546</v>
+        <v>130</v>
       </c>
       <c r="E1088" s="6" t="s">
         <v>19</v>
@@ -35560,51 +35598,51 @@
       </c>
       <c r="G1088" s="6"/>
       <c r="H1088" s="6" t="s">
-        <v>1547</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="1089" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1089" s="6"/>
       <c r="B1089" s="6" t="s">
-        <v>48</v>
+        <v>1545</v>
       </c>
       <c r="C1089" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1089" s="6" t="s">
-        <v>50</v>
+        <v>1546</v>
       </c>
       <c r="E1089" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1089" s="7" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="G1089" s="6"/>
       <c r="H1089" s="6" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="1090" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1090" s="6"/>
       <c r="B1090" s="6" t="s">
-        <v>552</v>
+        <v>48</v>
       </c>
       <c r="C1090" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1090" s="6" t="s">
-        <v>552</v>
+        <v>50</v>
       </c>
       <c r="E1090" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1090" s="7" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="G1090" s="6"/>
       <c r="H1090" s="6" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="1091" spans="1:8" x14ac:dyDescent="0.25">
@@ -35613,16 +35651,16 @@
         <v>552</v>
       </c>
       <c r="C1091" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1091" s="6" t="s">
-        <v>16</v>
+        <v>552</v>
       </c>
       <c r="E1091" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1091" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G1091" s="6"/>
       <c r="H1091" s="6" t="s">
@@ -35632,45 +35670,45 @@
     <row r="1092" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1092" s="6"/>
       <c r="B1092" s="6" t="s">
-        <v>23</v>
+        <v>552</v>
       </c>
       <c r="C1092" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1092" s="6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E1092" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1092" s="7" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="G1092" s="6"/>
       <c r="H1092" s="6" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="1093" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1093" s="6"/>
       <c r="B1093" s="6" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="C1093" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D1093" s="6" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="E1093" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1093" s="7" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="G1093" s="6"/>
       <c r="H1093" s="6" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="1094" spans="1:8" x14ac:dyDescent="0.25">
@@ -35679,16 +35717,16 @@
         <v>52</v>
       </c>
       <c r="C1094" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1094" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E1094" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1094" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G1094" s="6"/>
       <c r="H1094" s="6" t="s">
@@ -35698,44 +35736,44 @@
     <row r="1095" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1095" s="6"/>
       <c r="B1095" s="6" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C1095" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1095" s="6" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E1095" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1095" s="7" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="G1095" s="6"/>
-      <c r="H1095" s="6"/>
+      <c r="H1095" s="6" t="s">
+        <v>1551</v>
+      </c>
     </row>
     <row r="1096" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1096" s="6"/>
       <c r="B1096" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C1096" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1096" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E1096" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1096" s="7" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="G1096" s="6"/>
-      <c r="H1096" s="6" t="s">
-        <v>1552</v>
-      </c>
+      <c r="H1096" s="6"/>
     </row>
     <row r="1097" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1097" s="6"/>
@@ -35743,10 +35781,10 @@
         <v>66</v>
       </c>
       <c r="C1097" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1097" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E1097" s="6" t="s">
         <v>19</v>
@@ -35762,23 +35800,23 @@
     <row r="1098" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1098" s="6"/>
       <c r="B1098" s="6" t="s">
-        <v>415</v>
+        <v>66</v>
       </c>
       <c r="C1098" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1098" s="6" t="s">
-        <v>415</v>
+        <v>67</v>
       </c>
       <c r="E1098" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1098" s="7" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="G1098" s="6"/>
       <c r="H1098" s="6" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="1099" spans="1:8" x14ac:dyDescent="0.25">
@@ -35787,10 +35825,10 @@
         <v>415</v>
       </c>
       <c r="C1099" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1099" s="6" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="E1099" s="6" t="s">
         <v>19</v>
@@ -35806,133 +35844,133 @@
     <row r="1100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1100" s="6"/>
       <c r="B1100" s="6" t="s">
-        <v>1554</v>
+        <v>415</v>
       </c>
       <c r="C1100" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1100" s="6" t="s">
-        <v>1555</v>
+        <v>417</v>
       </c>
       <c r="E1100" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1100" s="7" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="G1100" s="6"/>
       <c r="H1100" s="6" t="s">
-        <v>1556</v>
+        <v>1553</v>
       </c>
     </row>
     <row r="1101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1101" s="6"/>
       <c r="B1101" s="6" t="s">
-        <v>70</v>
+        <v>1554</v>
       </c>
       <c r="C1101" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1101" s="6" t="s">
-        <v>71</v>
+        <v>1555</v>
       </c>
       <c r="E1101" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1101" s="12" t="s">
-        <v>72</v>
+        <v>19</v>
+      </c>
+      <c r="F1101" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="G1101" s="6"/>
       <c r="H1101" s="6" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="1102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1102" s="6"/>
       <c r="B1102" s="6" t="s">
-        <v>715</v>
+        <v>70</v>
       </c>
       <c r="C1102" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1102" s="6" t="s">
-        <v>716</v>
+        <v>71</v>
       </c>
       <c r="E1102" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1102" s="7" t="s">
-        <v>885</v>
+        <v>31</v>
+      </c>
+      <c r="F1102" s="12" t="s">
+        <v>72</v>
       </c>
       <c r="G1102" s="6"/>
       <c r="H1102" s="6" t="s">
-        <v>1550</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="1103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1103" s="6"/>
       <c r="B1103" s="6" t="s">
-        <v>1558</v>
+        <v>715</v>
       </c>
       <c r="C1103" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1103" s="6" t="s">
-        <v>1559</v>
+        <v>716</v>
       </c>
       <c r="E1103" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1103" s="7" t="s">
-        <v>56</v>
+        <v>885</v>
       </c>
       <c r="G1103" s="6"/>
       <c r="H1103" s="6" t="s">
-        <v>1560</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="1104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1104" s="6"/>
       <c r="B1104" s="6" t="s">
-        <v>91</v>
+        <v>1558</v>
       </c>
       <c r="C1104" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1104" s="6" t="s">
-        <v>91</v>
+        <v>1559</v>
       </c>
       <c r="E1104" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1104" s="7" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="G1104" s="6"/>
       <c r="H1104" s="6" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="1105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1105" s="6"/>
       <c r="B1105" s="6" t="s">
-        <v>271</v>
+        <v>91</v>
       </c>
       <c r="C1105" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D1105" s="6" t="s">
-        <v>271</v>
+        <v>91</v>
       </c>
       <c r="E1105" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1105" s="7" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="G1105" s="6"/>
       <c r="H1105" s="6" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="1106" spans="1:8" x14ac:dyDescent="0.25">
@@ -35941,16 +35979,16 @@
         <v>271</v>
       </c>
       <c r="C1106" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1106" s="6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E1106" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1106" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G1106" s="6"/>
       <c r="H1106" s="6" t="s">
@@ -35960,133 +35998,133 @@
     <row r="1107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1107" s="6"/>
       <c r="B1107" s="6" t="s">
-        <v>1563</v>
+        <v>271</v>
       </c>
       <c r="C1107" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1107" s="6" t="s">
-        <v>1564</v>
+        <v>273</v>
       </c>
       <c r="E1107" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1107" s="12" t="s">
-        <v>85</v>
+        <v>19</v>
+      </c>
+      <c r="F1107" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="G1107" s="6"/>
       <c r="H1107" s="6" t="s">
-        <v>1565</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="1108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1108" s="6"/>
       <c r="B1108" s="6" t="s">
-        <v>1566</v>
+        <v>1563</v>
       </c>
       <c r="C1108" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1108" s="6" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="E1108" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1108" s="7" t="s">
-        <v>614</v>
+        <v>31</v>
+      </c>
+      <c r="F1108" s="12" t="s">
+        <v>85</v>
       </c>
       <c r="G1108" s="6"/>
       <c r="H1108" s="6" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="1109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1109" s="6"/>
       <c r="B1109" s="6" t="s">
-        <v>193</v>
+        <v>1566</v>
       </c>
       <c r="C1109" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1109" s="6" t="s">
-        <v>194</v>
+        <v>1566</v>
       </c>
       <c r="E1109" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1109" s="12" t="s">
-        <v>60</v>
+        <v>19</v>
+      </c>
+      <c r="F1109" s="7" t="s">
+        <v>614</v>
       </c>
       <c r="G1109" s="6"/>
       <c r="H1109" s="6" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="1110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1110" s="6"/>
       <c r="B1110" s="6" t="s">
-        <v>1569</v>
+        <v>193</v>
       </c>
       <c r="C1110" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1110" s="6" t="s">
-        <v>1569</v>
+        <v>194</v>
       </c>
       <c r="E1110" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1110" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="F1110" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="G1110" s="6"/>
       <c r="H1110" s="6" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="1111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1111" s="6"/>
       <c r="B1111" s="6" t="s">
-        <v>215</v>
+        <v>1569</v>
       </c>
       <c r="C1111" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1111" s="6" t="s">
-        <v>217</v>
+        <v>1569</v>
       </c>
       <c r="E1111" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1111" s="7" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="G1111" s="6"/>
       <c r="H1111" s="6" t="s">
-        <v>431</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="1112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1112" s="6"/>
       <c r="B1112" s="6" t="s">
-        <v>108</v>
+        <v>215</v>
       </c>
       <c r="C1112" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1112" s="6" t="s">
-        <v>108</v>
+        <v>217</v>
       </c>
       <c r="E1112" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1112" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G1112" s="6"/>
       <c r="H1112" s="6" t="s">
-        <v>1561</v>
+        <v>431</v>
       </c>
     </row>
     <row r="1113" spans="1:8" x14ac:dyDescent="0.25">
@@ -36095,16 +36133,16 @@
         <v>108</v>
       </c>
       <c r="C1113" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1113" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E1113" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1113" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G1113" s="6"/>
       <c r="H1113" s="6" t="s">
@@ -36112,70 +36150,70 @@
       </c>
     </row>
     <row r="1114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1114" t="s">
+      <c r="A1114" s="6"/>
+      <c r="B1114" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1114" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1114" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1114" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1114" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1114" s="6"/>
+      <c r="H1114" s="6" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1115" t="s">
         <v>1571</v>
       </c>
     </row>
-    <row r="1115" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1115" s="6"/>
-      <c r="B1115" s="6" t="s">
-        <v>1572</v>
-      </c>
-      <c r="C1115" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1115" s="6" t="s">
-        <v>987</v>
-      </c>
-      <c r="E1115" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1115" s="7" t="s">
-        <v>1573</v>
-      </c>
-      <c r="G1115" s="6"/>
-      <c r="H1115" s="6" t="s">
-        <v>1574</v>
-      </c>
-    </row>
-    <row r="1116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1116" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1116" s="6"/>
       <c r="B1116" s="6" t="s">
-        <v>959</v>
+        <v>1572</v>
       </c>
       <c r="C1116" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1116" s="6" t="s">
-        <v>959</v>
+        <v>987</v>
       </c>
       <c r="E1116" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1116" s="7" t="s">
-        <v>23</v>
+        <v>1573</v>
       </c>
       <c r="G1116" s="6"/>
       <c r="H1116" s="6" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="1117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1117" s="6"/>
       <c r="B1117" s="6" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="C1117" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1117" s="6" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="E1117" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1117" s="7" t="s">
-        <v>98</v>
+        <v>23</v>
       </c>
       <c r="G1117" s="6"/>
       <c r="H1117" s="6" t="s">
@@ -36185,41 +36223,41 @@
     <row r="1118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1118" s="6"/>
       <c r="B1118" s="6" t="s">
-        <v>127</v>
+        <v>961</v>
       </c>
       <c r="C1118" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1118" s="6" t="s">
-        <v>127</v>
+        <v>962</v>
       </c>
       <c r="E1118" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1118" s="7" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="G1118" s="6"/>
       <c r="H1118" s="6" t="s">
-        <v>996</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="1119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1119" s="6"/>
       <c r="B1119" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C1119" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1119" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E1119" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1119" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G1119" s="6"/>
       <c r="H1119" s="6" t="s">
@@ -36229,111 +36267,111 @@
     <row r="1120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1120" s="6"/>
       <c r="B1120" s="6" t="s">
-        <v>34</v>
+        <v>129</v>
       </c>
       <c r="C1120" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1120" s="6" t="s">
-        <v>34</v>
+        <v>130</v>
       </c>
       <c r="E1120" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1120" s="7" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="G1120" s="6"/>
       <c r="H1120" s="6" t="s">
-        <v>1576</v>
+        <v>996</v>
       </c>
     </row>
     <row r="1121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1121" s="6"/>
       <c r="B1121" s="6" t="s">
-        <v>1577</v>
+        <v>34</v>
       </c>
       <c r="C1121" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D1121" s="6" t="s">
-        <v>1577</v>
+        <v>34</v>
       </c>
       <c r="E1121" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1121" s="7" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="G1121" s="6"/>
       <c r="H1121" s="6" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="1122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1122" s="6"/>
       <c r="B1122" s="6" t="s">
-        <v>37</v>
+        <v>1577</v>
       </c>
       <c r="C1122" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1122" s="6" t="s">
-        <v>38</v>
+        <v>1577</v>
       </c>
       <c r="E1122" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1122" s="7" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="G1122" s="6"/>
       <c r="H1122" s="6" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="1123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1123" s="6"/>
       <c r="B1123" s="6" t="s">
-        <v>325</v>
+        <v>37</v>
       </c>
       <c r="C1123" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1123" s="6" t="s">
-        <v>326</v>
+        <v>38</v>
       </c>
       <c r="E1123" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1123" s="7" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="G1123" s="6"/>
       <c r="H1123" s="6" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="1124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1124" s="6"/>
       <c r="B1124" s="6" t="s">
-        <v>39</v>
+        <v>325</v>
       </c>
       <c r="C1124" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1124" s="6" t="s">
-        <v>39</v>
+        <v>326</v>
       </c>
       <c r="E1124" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1124" s="7" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="G1124" s="6"/>
       <c r="H1124" s="6" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="1125" spans="1:8" x14ac:dyDescent="0.25">
@@ -36342,10 +36380,10 @@
         <v>39</v>
       </c>
       <c r="C1125" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1125" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E1125" s="6" t="s">
         <v>19</v>
@@ -36361,41 +36399,41 @@
     <row r="1126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1126" s="6"/>
       <c r="B1126" s="6" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C1126" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1126" s="6" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E1126" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1126" s="12" t="s">
-        <v>60</v>
+        <v>19</v>
+      </c>
+      <c r="F1126" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="G1126" s="6"/>
       <c r="H1126" s="6" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="1127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1127" s="6"/>
       <c r="B1127" s="6" t="s">
-        <v>1583</v>
+        <v>48</v>
       </c>
       <c r="C1127" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1127" s="6" t="s">
-        <v>1583</v>
+        <v>50</v>
       </c>
       <c r="E1127" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1127" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="F1127" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="G1127" s="6"/>
       <c r="H1127" s="6" t="s">
@@ -36405,19 +36443,19 @@
     <row r="1128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1128" s="6"/>
       <c r="B1128" s="6" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="C1128" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D1128" s="6" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="E1128" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1128" s="7" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="G1128" s="6"/>
       <c r="H1128" s="6" t="s">
@@ -36427,45 +36465,45 @@
     <row r="1129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1129" s="6"/>
       <c r="B1129" s="6" t="s">
-        <v>964</v>
+        <v>1584</v>
       </c>
       <c r="C1129" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1129" s="6" t="s">
-        <v>965</v>
+        <v>1584</v>
       </c>
       <c r="E1129" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1129" s="7" t="s">
-        <v>452</v>
+        <v>53</v>
       </c>
       <c r="G1129" s="6"/>
       <c r="H1129" s="6" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="1130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1130" s="6"/>
       <c r="B1130" s="6" t="s">
-        <v>52</v>
+        <v>964</v>
       </c>
       <c r="C1130" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1130" s="6" t="s">
-        <v>52</v>
+        <v>965</v>
       </c>
       <c r="E1130" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1130" s="7" t="s">
-        <v>53</v>
+        <v>452</v>
       </c>
       <c r="G1130" s="6"/>
       <c r="H1130" s="6" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="1131" spans="1:8" x14ac:dyDescent="0.25">
@@ -36474,32 +36512,32 @@
         <v>52</v>
       </c>
       <c r="C1131" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1131" s="6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E1131" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1131" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G1131" s="6"/>
       <c r="H1131" s="6" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="1132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1132" s="6"/>
       <c r="B1132" s="6" t="s">
-        <v>394</v>
+        <v>52</v>
       </c>
       <c r="C1132" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1132" s="6" t="s">
-        <v>396</v>
+        <v>55</v>
       </c>
       <c r="E1132" s="6" t="s">
         <v>19</v>
@@ -36509,50 +36547,50 @@
       </c>
       <c r="G1132" s="6"/>
       <c r="H1132" s="6" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="1133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1133" s="6"/>
       <c r="B1133" s="6" t="s">
-        <v>64</v>
+        <v>394</v>
       </c>
       <c r="C1133" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1133" s="6" t="s">
-        <v>65</v>
+        <v>396</v>
       </c>
       <c r="E1133" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1133" s="7" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="G1133" s="6"/>
-      <c r="H1133" s="6"/>
+      <c r="H1133" s="6" t="s">
+        <v>1588</v>
+      </c>
     </row>
     <row r="1134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1134" s="6"/>
       <c r="B1134" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C1134" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1134" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E1134" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1134" s="7" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="G1134" s="6"/>
-      <c r="H1134" s="6" t="s">
-        <v>1589</v>
-      </c>
+      <c r="H1134" s="6"/>
     </row>
     <row r="1135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1135" s="6"/>
@@ -36560,10 +36598,10 @@
         <v>66</v>
       </c>
       <c r="C1135" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1135" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E1135" s="6" t="s">
         <v>19</v>
@@ -36579,133 +36617,133 @@
     <row r="1136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1136" s="6"/>
       <c r="B1136" s="6" t="s">
-        <v>778</v>
+        <v>66</v>
       </c>
       <c r="C1136" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1136" s="6" t="s">
-        <v>778</v>
+        <v>67</v>
       </c>
       <c r="E1136" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1136" s="7" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="G1136" s="6"/>
       <c r="H1136" s="6" t="s">
-        <v>779</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="1137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1137" s="6"/>
       <c r="B1137" s="6" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="C1137" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D1137" s="6" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="E1137" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1137" s="7" t="s">
-        <v>366</v>
+        <v>53</v>
       </c>
       <c r="G1137" s="6"/>
       <c r="H1137" s="6" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="1138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1138" s="6"/>
       <c r="B1138" s="6" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C1138" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1138" s="6" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="E1138" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1138" s="7" t="s">
-        <v>784</v>
+        <v>366</v>
       </c>
       <c r="G1138" s="6"/>
       <c r="H1138" s="6" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
     </row>
     <row r="1139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1139" s="6"/>
       <c r="B1139" s="6" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="C1139" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1139" s="6" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="E1139" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1139" s="7" t="s">
-        <v>366</v>
+        <v>784</v>
       </c>
       <c r="G1139" s="6"/>
       <c r="H1139" s="6" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="1140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1140" s="6"/>
       <c r="B1140" s="6" t="s">
-        <v>1008</v>
+        <v>785</v>
       </c>
       <c r="C1140" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1140" s="6" t="s">
-        <v>1010</v>
+        <v>786</v>
       </c>
       <c r="E1140" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1140" s="7" t="s">
-        <v>56</v>
+        <v>366</v>
       </c>
       <c r="G1140" s="6"/>
       <c r="H1140" s="6" t="s">
-        <v>1009</v>
+        <v>781</v>
       </c>
     </row>
     <row r="1141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1141" s="6"/>
       <c r="B1141" s="6" t="s">
-        <v>787</v>
+        <v>1008</v>
       </c>
       <c r="C1141" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1141" s="6" t="s">
-        <v>787</v>
+        <v>1010</v>
       </c>
       <c r="E1141" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1141" s="7" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G1141" s="6"/>
       <c r="H1141" s="6" t="s">
-        <v>1590</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="1142" spans="1:8" x14ac:dyDescent="0.25">
@@ -36714,10 +36752,10 @@
         <v>787</v>
       </c>
       <c r="C1142" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1142" s="6" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="E1142" s="6" t="s">
         <v>19</v>
@@ -36733,177 +36771,177 @@
     <row r="1143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1143" s="6"/>
       <c r="B1143" s="6" t="s">
-        <v>166</v>
+        <v>787</v>
       </c>
       <c r="C1143" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1143" s="6" t="s">
-        <v>168</v>
+        <v>789</v>
       </c>
       <c r="E1143" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1143" s="12" t="s">
-        <v>60</v>
+        <v>19</v>
+      </c>
+      <c r="F1143" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="G1143" s="6"/>
       <c r="H1143" s="6" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="1144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1144" s="6"/>
       <c r="B1144" s="6" t="s">
-        <v>70</v>
+        <v>166</v>
       </c>
       <c r="C1144" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1144" s="6" t="s">
-        <v>71</v>
+        <v>168</v>
       </c>
       <c r="E1144" s="6" t="s">
         <v>31</v>
       </c>
       <c r="F1144" s="12" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="G1144" s="6"/>
       <c r="H1144" s="6" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="1145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1145" s="6"/>
       <c r="B1145" s="6" t="s">
-        <v>839</v>
+        <v>70</v>
       </c>
       <c r="C1145" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1145" s="6" t="s">
-        <v>839</v>
+        <v>71</v>
       </c>
       <c r="E1145" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1145" s="7" t="s">
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="F1145" s="12" t="s">
+        <v>72</v>
       </c>
       <c r="G1145" s="6"/>
       <c r="H1145" s="6" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="1146" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1146" s="6"/>
       <c r="B1146" s="6" t="s">
-        <v>715</v>
+        <v>839</v>
       </c>
       <c r="C1146" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1146" s="6" t="s">
-        <v>716</v>
+        <v>839</v>
       </c>
       <c r="E1146" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1146" s="7" t="s">
-        <v>717</v>
+        <v>23</v>
       </c>
       <c r="G1146" s="6"/>
       <c r="H1146" s="6" t="s">
         <v>1004</v>
       </c>
     </row>
-    <row r="1147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1147" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1147" s="6"/>
       <c r="B1147" s="6" t="s">
-        <v>1593</v>
+        <v>715</v>
       </c>
       <c r="C1147" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1147" s="6" t="s">
-        <v>1594</v>
+        <v>716</v>
       </c>
       <c r="E1147" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1147" s="12" t="s">
-        <v>85</v>
+        <v>19</v>
+      </c>
+      <c r="F1147" s="7" t="s">
+        <v>717</v>
       </c>
       <c r="G1147" s="6"/>
       <c r="H1147" s="6" t="s">
-        <v>1595</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="1148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1148" s="6"/>
       <c r="B1148" s="6" t="s">
-        <v>91</v>
+        <v>1593</v>
       </c>
       <c r="C1148" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1148" s="6" t="s">
-        <v>91</v>
+        <v>1594</v>
       </c>
       <c r="E1148" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1148" s="7" t="s">
-        <v>92</v>
+        <v>31</v>
+      </c>
+      <c r="F1148" s="12" t="s">
+        <v>85</v>
       </c>
       <c r="G1148" s="6"/>
       <c r="H1148" s="6" t="s">
-        <v>1526</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="1149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1149" s="6"/>
       <c r="B1149" s="6" t="s">
-        <v>1596</v>
+        <v>91</v>
       </c>
       <c r="C1149" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1149" s="6" t="s">
-        <v>1597</v>
+        <v>91</v>
       </c>
       <c r="E1149" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1149" s="12" t="s">
-        <v>85</v>
+        <v>19</v>
+      </c>
+      <c r="F1149" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="G1149" s="6"/>
       <c r="H1149" s="6" t="s">
-        <v>1598</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="1150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1150" s="6"/>
       <c r="B1150" s="6" t="s">
-        <v>271</v>
+        <v>1596</v>
       </c>
       <c r="C1150" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1150" s="6" t="s">
-        <v>271</v>
+        <v>1597</v>
       </c>
       <c r="E1150" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1150" s="7" t="s">
-        <v>53</v>
+        <v>31</v>
+      </c>
+      <c r="F1150" s="12" t="s">
+        <v>85</v>
       </c>
       <c r="G1150" s="6"/>
       <c r="H1150" s="6" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="1151" spans="1:8" x14ac:dyDescent="0.25">
@@ -36912,16 +36950,16 @@
         <v>271</v>
       </c>
       <c r="C1151" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1151" s="6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E1151" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1151" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G1151" s="6"/>
       <c r="H1151" s="6" t="s">
@@ -36931,35 +36969,35 @@
     <row r="1152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1152" s="6"/>
       <c r="B1152" s="6" t="s">
-        <v>1600</v>
+        <v>271</v>
       </c>
       <c r="C1152" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1152" s="6" t="s">
-        <v>1600</v>
+        <v>273</v>
       </c>
       <c r="E1152" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1152" s="7" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="G1152" s="6"/>
       <c r="H1152" s="6" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="1153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1153" s="6"/>
       <c r="B1153" s="6" t="s">
-        <v>1449</v>
+        <v>1600</v>
       </c>
       <c r="C1153" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1153" s="6" t="s">
-        <v>1450</v>
+        <v>1600</v>
       </c>
       <c r="E1153" s="6" t="s">
         <v>19</v>
@@ -36975,23 +37013,23 @@
     <row r="1154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1154" s="6"/>
       <c r="B1154" s="6" t="s">
-        <v>190</v>
+        <v>1449</v>
       </c>
       <c r="C1154" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1154" s="6" t="s">
-        <v>190</v>
+        <v>1450</v>
       </c>
       <c r="E1154" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1154" s="7" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="G1154" s="6"/>
       <c r="H1154" s="6" t="s">
-        <v>940</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="1155" spans="1:8" x14ac:dyDescent="0.25">
@@ -37000,10 +37038,10 @@
         <v>190</v>
       </c>
       <c r="C1155" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1155" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E1155" s="6" t="s">
         <v>19</v>
@@ -37019,89 +37057,89 @@
     <row r="1156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1156" s="6"/>
       <c r="B1156" s="6" t="s">
-        <v>1602</v>
+        <v>190</v>
       </c>
       <c r="C1156" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1156" s="6" t="s">
-        <v>242</v>
+        <v>191</v>
       </c>
       <c r="E1156" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1156" s="7" t="s">
-        <v>1603</v>
+        <v>48</v>
       </c>
       <c r="G1156" s="6"/>
       <c r="H1156" s="6" t="s">
-        <v>1604</v>
+        <v>940</v>
       </c>
     </row>
     <row r="1157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1157" s="6"/>
       <c r="B1157" s="6" t="s">
-        <v>193</v>
+        <v>1602</v>
       </c>
       <c r="C1157" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1157" s="6" t="s">
-        <v>194</v>
+        <v>242</v>
       </c>
       <c r="E1157" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1157" s="12" t="s">
-        <v>60</v>
+        <v>19</v>
+      </c>
+      <c r="F1157" s="7" t="s">
+        <v>1603</v>
       </c>
       <c r="G1157" s="6"/>
       <c r="H1157" s="6" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="1158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1158" s="6"/>
       <c r="B1158" s="6" t="s">
-        <v>1026</v>
+        <v>193</v>
       </c>
       <c r="C1158" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1158" s="6" t="s">
-        <v>1027</v>
+        <v>194</v>
       </c>
       <c r="E1158" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1158" s="7" t="s">
-        <v>56</v>
+        <v>31</v>
+      </c>
+      <c r="F1158" s="12" t="s">
+        <v>60</v>
       </c>
       <c r="G1158" s="6"/>
       <c r="H1158" s="6" t="s">
-        <v>1028</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="1159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1159" s="6"/>
       <c r="B1159" s="6" t="s">
-        <v>793</v>
+        <v>1026</v>
       </c>
       <c r="C1159" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1159" s="6" t="s">
-        <v>793</v>
+        <v>1027</v>
       </c>
       <c r="E1159" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1159" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G1159" s="6"/>
       <c r="H1159" s="6" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="1160" spans="1:8" x14ac:dyDescent="0.25">
@@ -37110,16 +37148,16 @@
         <v>793</v>
       </c>
       <c r="C1160" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1160" s="6" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="E1160" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1160" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G1160" s="6"/>
       <c r="H1160" s="6" t="s">
@@ -37129,23 +37167,23 @@
     <row r="1161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1161" s="6"/>
       <c r="B1161" s="6" t="s">
-        <v>982</v>
+        <v>793</v>
       </c>
       <c r="C1161" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1161" s="6" t="s">
-        <v>982</v>
+        <v>795</v>
       </c>
       <c r="E1161" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1161" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G1161" s="6"/>
       <c r="H1161" s="6" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="1162" spans="1:8" x14ac:dyDescent="0.25">
@@ -37154,16 +37192,16 @@
         <v>982</v>
       </c>
       <c r="C1162" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1162" s="6" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="E1162" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1162" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G1162" s="6"/>
       <c r="H1162" s="6" t="s">
@@ -37173,23 +37211,23 @@
     <row r="1163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1163" s="6"/>
       <c r="B1163" s="6" t="s">
-        <v>1606</v>
+        <v>982</v>
       </c>
       <c r="C1163" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1163" s="6" t="s">
-        <v>1606</v>
+        <v>984</v>
       </c>
       <c r="E1163" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1163" s="7" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="G1163" s="6"/>
       <c r="H1163" s="6" t="s">
-        <v>1607</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="1164" spans="1:8" x14ac:dyDescent="0.25">
@@ -37198,10 +37236,10 @@
         <v>1606</v>
       </c>
       <c r="C1164" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1164" s="6" t="s">
-        <v>1608</v>
+        <v>1606</v>
       </c>
       <c r="E1164" s="6" t="s">
         <v>19</v>
@@ -37217,23 +37255,23 @@
     <row r="1165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1165" s="6"/>
       <c r="B1165" s="6" t="s">
-        <v>427</v>
+        <v>1606</v>
       </c>
       <c r="C1165" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1165" s="6" t="s">
-        <v>427</v>
+        <v>1608</v>
       </c>
       <c r="E1165" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1165" s="7" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="G1165" s="6"/>
       <c r="H1165" s="6" t="s">
-        <v>1609</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="1166" spans="1:8" x14ac:dyDescent="0.25">
@@ -37242,42 +37280,42 @@
         <v>427</v>
       </c>
       <c r="C1166" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1166" s="6" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E1166" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1166" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G1166" s="6"/>
       <c r="H1166" s="6" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="1167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1167" s="6"/>
       <c r="B1167" s="6" t="s">
-        <v>215</v>
+        <v>427</v>
       </c>
       <c r="C1167" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1167" s="6" t="s">
-        <v>215</v>
+        <v>429</v>
       </c>
       <c r="E1167" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1167" s="7" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G1167" s="6"/>
       <c r="H1167" s="6" t="s">
-        <v>796</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="1168" spans="1:8" x14ac:dyDescent="0.25">
@@ -37286,10 +37324,10 @@
         <v>215</v>
       </c>
       <c r="C1168" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1168" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E1168" s="6" t="s">
         <v>19</v>
@@ -37305,23 +37343,23 @@
     <row r="1169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1169" s="6"/>
       <c r="B1169" s="6" t="s">
-        <v>108</v>
+        <v>215</v>
       </c>
       <c r="C1169" s="6" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D1169" s="6" t="s">
-        <v>108</v>
+        <v>217</v>
       </c>
       <c r="E1169" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1169" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G1169" s="6"/>
       <c r="H1169" s="6" t="s">
-        <v>1537</v>
+        <v>796</v>
       </c>
     </row>
     <row r="1170" spans="1:8" x14ac:dyDescent="0.25">
@@ -37330,41 +37368,63 @@
         <v>108</v>
       </c>
       <c r="C1170" s="6" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D1170" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E1170" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F1170" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G1170" s="6"/>
       <c r="H1170" s="6" t="s">
-        <v>1611</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="1171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1171" s="6"/>
       <c r="B1171" s="6" t="s">
-        <v>743</v>
+        <v>108</v>
       </c>
       <c r="C1171" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D1171" s="6" t="s">
-        <v>744</v>
+        <v>109</v>
       </c>
       <c r="E1171" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1171" s="12" t="s">
-        <v>60</v>
+        <v>19</v>
+      </c>
+      <c r="F1171" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="G1171" s="6"/>
       <c r="H1171" s="6" t="s">
+        <v>1611</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1172" s="6"/>
+      <c r="B1172" s="6" t="s">
+        <v>743</v>
+      </c>
+      <c r="C1172" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1172" s="6" t="s">
+        <v>744</v>
+      </c>
+      <c r="E1172" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1172" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1172" s="6"/>
+      <c r="H1172" s="6" t="s">
         <v>1034</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Renamed "# of participants" to "# Subjects"
</commit_message>
<xml_diff>
--- a/src/conf/xlsx/column-and-parameter-descriptions-R5.xlsx
+++ b/src/conf/xlsx/column-and-parameter-descriptions-R5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\lhc-lx-sedinkinya\sedinkinya\Projects\fhir-obs-viewer\src\conf\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9B4076-969B-4FF1-B5B5-3EDE1588AC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA2C113-FEE1-4DFA-957E-10CFEF22629D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6570" yWindow="2865" windowWidth="38700" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6570" yWindow="2865" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources on LForms R5 server" sheetId="1" r:id="rId1"/>
@@ -4874,10 +4874,10 @@
     <t>unsignedInt</t>
   </si>
   <si>
-    <t># of participants</t>
-  </si>
-  <si>
     <t>recruitment.actualNumber</t>
+  </si>
+  <si>
+    <t># Subjects</t>
   </si>
 </sst>
 </file>
@@ -5294,8 +5294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H329"/>
   <sheetViews>
-    <sheetView topLeftCell="A294" workbookViewId="0">
-      <selection activeCell="A312" sqref="A312:XFD312"/>
+    <sheetView tabSelected="1" topLeftCell="A294" workbookViewId="0">
+      <selection activeCell="D312" sqref="D312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -11870,7 +11870,7 @@
         <v>29</v>
       </c>
       <c r="D312" s="2" t="s">
-        <v>1617</v>
+        <v>1618</v>
       </c>
       <c r="E312" s="2" t="s">
         <v>19</v>
@@ -11879,7 +11879,7 @@
         <v>1616</v>
       </c>
       <c r="G312" s="2" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="H312" s="2" t="s">
         <v>1615</v>
@@ -12268,8 +12268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1042" workbookViewId="0">
-      <selection activeCell="G1069" sqref="G1069"/>
+    <sheetView topLeftCell="A1048" workbookViewId="0">
+      <selection activeCell="D1069" sqref="D1069"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -35185,7 +35185,7 @@
         <v>29</v>
       </c>
       <c r="D1069" s="2" t="s">
-        <v>1617</v>
+        <v>1618</v>
       </c>
       <c r="E1069" s="2" t="s">
         <v>19</v>
@@ -35194,7 +35194,7 @@
         <v>1616</v>
       </c>
       <c r="G1069" s="2" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="H1069" s="2" t="s">
         <v>1615</v>

</xml_diff>

<commit_message>
Changes as per review
LF-3262
</commit_message>
<xml_diff>
--- a/src/conf/xlsx/column-and-parameter-descriptions-R5.xlsx
+++ b/src/conf/xlsx/column-and-parameter-descriptions-R5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\lhc-lx-sedinkinya\sedinkinya\Projects\fhir-obs-viewer\src\conf\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\lhc-lx-ftdev04\sedinkinya\Projects\fhir-obs-viewer\src\conf\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA2C113-FEE1-4DFA-957E-10CFEF22629D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39D3120-5C66-4556-8FCB-C188C30A0A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6570" yWindow="2865" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3915" yWindow="2880" windowWidth="38700" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources on LForms R5 server" sheetId="1" r:id="rId1"/>
@@ -4996,9 +4996,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5036,7 +5036,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5142,7 +5142,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5284,7 +5284,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5294,8 +5294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H329"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A294" workbookViewId="0">
-      <selection activeCell="D312" sqref="D312"/>
+    <sheetView topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="F128" sqref="F128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5726,7 +5726,7 @@
       <c r="E28" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="F28" s="9" t="s">
         <v>60</v>
       </c>
       <c r="G28" s="8"/>
@@ -7223,7 +7223,7 @@
       <c r="E97" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F97" s="12" t="s">
+      <c r="F97" s="9" t="s">
         <v>60</v>
       </c>
       <c r="G97" s="8"/>
@@ -7884,9 +7884,9 @@
         <v>263</v>
       </c>
       <c r="E128" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F128" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F128" s="11" t="s">
         <v>60</v>
       </c>
       <c r="G128" s="10"/>
@@ -7930,7 +7930,7 @@
       <c r="E130" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F130" s="12" t="s">
+      <c r="F130" s="9" t="s">
         <v>60</v>
       </c>
       <c r="G130" s="8"/>
@@ -11239,7 +11239,7 @@
       <c r="E283" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F283" s="12" t="s">
+      <c r="F283" s="9" t="s">
         <v>60</v>
       </c>
       <c r="G283" s="8"/>
@@ -12268,8 +12268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H1172"/>
   <sheetViews>
-    <sheetView topLeftCell="A1048" workbookViewId="0">
-      <selection activeCell="D1069" sqref="D1069"/>
+    <sheetView tabSelected="1" topLeftCell="A1147" workbookViewId="0">
+      <selection activeCell="F1172" sqref="F1172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13868,9 +13868,9 @@
         <v>756</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F79" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F79" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G79" s="6"/>
@@ -15057,9 +15057,9 @@
         <v>194</v>
       </c>
       <c r="E134" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F134" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F134" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G134" s="6"/>
@@ -15852,9 +15852,9 @@
         <v>858</v>
       </c>
       <c r="E171" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F171" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F171" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G171" s="6"/>
@@ -16006,9 +16006,9 @@
         <v>868</v>
       </c>
       <c r="E178" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F178" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F178" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G178" s="6"/>
@@ -17398,9 +17398,9 @@
         <v>194</v>
       </c>
       <c r="E243" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F243" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F243" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G243" s="6"/>
@@ -18347,9 +18347,9 @@
         <v>194</v>
       </c>
       <c r="E287" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F287" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F287" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G287" s="6"/>
@@ -18946,9 +18946,9 @@
         <v>59</v>
       </c>
       <c r="E315" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F315" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F315" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G315" s="6"/>
@@ -19631,9 +19631,9 @@
         <v>50</v>
       </c>
       <c r="E347" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F347" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F347" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G347" s="6"/>
@@ -20157,9 +20157,9 @@
         <v>273</v>
       </c>
       <c r="E371" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F371" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F371" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G371" s="6"/>
@@ -20267,9 +20267,9 @@
         <v>194</v>
       </c>
       <c r="E376" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F376" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F376" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G376" s="6"/>
@@ -21507,9 +21507,9 @@
         <v>38</v>
       </c>
       <c r="E434" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F434" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F434" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G434" s="6"/>
@@ -21881,9 +21881,9 @@
         <v>1118</v>
       </c>
       <c r="E451" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F451" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F451" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G451" s="6"/>
@@ -23598,9 +23598,9 @@
         <v>205</v>
       </c>
       <c r="E530" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F530" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F530" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G530" s="6"/>
@@ -24594,9 +24594,9 @@
         <v>719</v>
       </c>
       <c r="E577" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F577" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F577" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G577" s="6"/>
@@ -25147,9 +25147,9 @@
         <v>194</v>
       </c>
       <c r="E603" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F603" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F603" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G603" s="6"/>
@@ -27339,9 +27339,9 @@
         <v>387</v>
       </c>
       <c r="E706" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F706" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F706" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G706" s="6"/>
@@ -27557,9 +27557,9 @@
         <v>263</v>
       </c>
       <c r="E716" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F716" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F716" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G716" s="6"/>
@@ -27733,9 +27733,9 @@
         <v>194</v>
       </c>
       <c r="E724" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F724" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F724" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G724" s="6"/>
@@ -28418,9 +28418,9 @@
         <v>263</v>
       </c>
       <c r="E756" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F756" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F756" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G756" s="6"/>
@@ -28462,9 +28462,9 @@
         <v>267</v>
       </c>
       <c r="E758" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F758" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F758" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G758" s="6"/>
@@ -29215,9 +29215,9 @@
         <v>387</v>
       </c>
       <c r="E793" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F793" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F793" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G793" s="6"/>
@@ -29675,9 +29675,9 @@
         <v>263</v>
       </c>
       <c r="E814" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F814" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F814" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G814" s="6"/>
@@ -29851,9 +29851,9 @@
         <v>194</v>
       </c>
       <c r="E822" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F822" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F822" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G822" s="6"/>
@@ -30536,9 +30536,9 @@
         <v>263</v>
       </c>
       <c r="E854" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F854" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F854" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G854" s="6"/>
@@ -30624,9 +30624,9 @@
         <v>194</v>
       </c>
       <c r="E858" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F858" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F858" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G858" s="6"/>
@@ -33427,9 +33427,9 @@
         <v>1509</v>
       </c>
       <c r="E988" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F988" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F988" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G988" s="6"/>
@@ -33953,9 +33953,9 @@
         <v>194</v>
       </c>
       <c r="E1012" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1012" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1012" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G1012" s="6"/>
@@ -34261,9 +34261,9 @@
         <v>1541</v>
       </c>
       <c r="E1026" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1026" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1026" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G1026" s="6"/>
@@ -34552,9 +34552,9 @@
         <v>396</v>
       </c>
       <c r="E1040" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1040" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1040" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G1040" s="6"/>
@@ -36073,9 +36073,9 @@
         <v>194</v>
       </c>
       <c r="E1110" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1110" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1110" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G1110" s="6"/>
@@ -36430,9 +36430,9 @@
         <v>50</v>
       </c>
       <c r="E1127" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1127" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1127" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G1127" s="6"/>
@@ -36802,9 +36802,9 @@
         <v>168</v>
       </c>
       <c r="E1144" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1144" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1144" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G1144" s="6"/>
@@ -37110,9 +37110,9 @@
         <v>194</v>
       </c>
       <c r="E1158" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1158" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1158" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G1158" s="6"/>
@@ -37418,9 +37418,9 @@
         <v>744</v>
       </c>
       <c r="E1172" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1172" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1172" s="7" t="s">
         <v>60</v>
       </c>
       <c r="G1172" s="6"/>

</xml_diff>